<commit_message>
Update cervical cancer intervention data - 350 and 351
</commit_message>
<xml_diff>
--- a/2_data/new_intervention_names.xlsx
+++ b/2_data/new_intervention_names.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="441">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="443">
   <si>
     <t>Category</t>
   </si>
@@ -1350,6 +1350,12 @@
   </si>
   <si>
     <t>Basic psychosocial support, advice, and follow-up (including antidepressants)</t>
+  </si>
+  <si>
+    <t>Smear test at age 40 fo cervical cancer detection + cancer treatment</t>
+  </si>
+  <si>
+    <t>Smear test at age 40 fo cervical cancer detection + HPV vaccinations starting at age 12 + cancer treatment</t>
   </si>
 </sst>
 </file>
@@ -1697,10 +1703,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I142"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:I144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="C114" sqref="C114"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F145" sqref="F145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1732,7 +1739,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1753,7 +1760,7 @@
       </c>
       <c r="H2"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1774,7 +1781,7 @@
       </c>
       <c r="H3"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1795,7 +1802,7 @@
       </c>
       <c r="H4"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1816,7 +1823,7 @@
       </c>
       <c r="H5"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -1837,7 +1844,7 @@
       </c>
       <c r="H6"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -1858,7 +1865,7 @@
       </c>
       <c r="H7"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -1879,7 +1886,7 @@
       </c>
       <c r="H8"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -1900,7 +1907,7 @@
       </c>
       <c r="H9"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -1921,7 +1928,7 @@
       </c>
       <c r="H10"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -1945,7 +1952,7 @@
       </c>
       <c r="H11"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -1966,7 +1973,7 @@
       </c>
       <c r="H12"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -1987,7 +1994,7 @@
       </c>
       <c r="H13"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -2008,7 +2015,7 @@
       </c>
       <c r="H14"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -2029,7 +2036,7 @@
       </c>
       <c r="H15"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -2050,7 +2057,7 @@
       </c>
       <c r="H16"/>
     </row>
-    <row r="17" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>3</v>
       </c>
@@ -2070,7 +2077,7 @@
         <v>12.287983160102591</v>
       </c>
     </row>
-    <row r="18" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>3</v>
       </c>
@@ -2090,7 +2097,7 @@
         <v>5.8764426199980653</v>
       </c>
     </row>
-    <row r="19" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>3</v>
       </c>
@@ -2110,7 +2117,7 @@
         <v>22.626927498876491</v>
       </c>
     </row>
-    <row r="20" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>3</v>
       </c>
@@ -2130,7 +2137,7 @@
         <v>22.626927498876483</v>
       </c>
     </row>
-    <row r="21" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>3</v>
       </c>
@@ -2150,7 +2157,7 @@
         <v>4.810820102639263</v>
       </c>
     </row>
-    <row r="22" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>3</v>
       </c>
@@ -2170,7 +2177,7 @@
         <v>43.937776702649238</v>
       </c>
     </row>
-    <row r="23" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>3</v>
       </c>
@@ -2190,7 +2197,7 @@
         <v>69.987315823932676</v>
       </c>
     </row>
-    <row r="24" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>3</v>
       </c>
@@ -2210,7 +2217,7 @@
         <v>3.0761982466467503</v>
       </c>
     </row>
-    <row r="25" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>3</v>
       </c>
@@ -2230,7 +2237,7 @@
         <v>68.864561953102353</v>
       </c>
     </row>
-    <row r="26" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>3</v>
       </c>
@@ -2250,7 +2257,7 @@
         <v>36.727766374987922</v>
       </c>
     </row>
-    <row r="27" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>3</v>
       </c>
@@ -2270,7 +2277,7 @@
         <v>19.248450535311211</v>
       </c>
     </row>
-    <row r="28" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>56</v>
       </c>
@@ -2290,7 +2297,7 @@
         <v>17.768996830715984</v>
       </c>
     </row>
-    <row r="29" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>56</v>
       </c>
@@ -2310,7 +2317,7 @@
         <v>17.768996830715984</v>
       </c>
     </row>
-    <row r="30" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>56</v>
       </c>
@@ -2330,7 +2337,7 @@
         <v>17.768996830715984</v>
       </c>
     </row>
-    <row r="31" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>56</v>
       </c>
@@ -2350,7 +2357,7 @@
         <v>17.768996830715988</v>
       </c>
     </row>
-    <row r="32" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>65</v>
       </c>
@@ -2370,7 +2377,7 @@
         <v>60.706723287675047</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>65</v>
       </c>
@@ -2391,7 +2398,7 @@
       </c>
       <c r="H33"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>65</v>
       </c>
@@ -2412,7 +2419,7 @@
       </c>
       <c r="H34"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>65</v>
       </c>
@@ -2433,7 +2440,7 @@
       </c>
       <c r="H35"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>65</v>
       </c>
@@ -2454,7 +2461,7 @@
       </c>
       <c r="H36"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>65</v>
       </c>
@@ -2475,7 +2482,7 @@
       </c>
       <c r="H37"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>65</v>
       </c>
@@ -2496,7 +2503,7 @@
       </c>
       <c r="H38"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>65</v>
       </c>
@@ -2569,7 +2576,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>65</v>
       </c>
@@ -2590,7 +2597,7 @@
       </c>
       <c r="H42"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>88</v>
       </c>
@@ -2611,7 +2618,7 @@
       </c>
       <c r="H43"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>88</v>
       </c>
@@ -2632,7 +2639,7 @@
       </c>
       <c r="H44"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>88</v>
       </c>
@@ -2653,7 +2660,7 @@
       </c>
       <c r="H45"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>88</v>
       </c>
@@ -2674,7 +2681,7 @@
       </c>
       <c r="H46"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>88</v>
       </c>
@@ -2695,7 +2702,7 @@
       </c>
       <c r="H47"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>88</v>
       </c>
@@ -2716,7 +2723,7 @@
       </c>
       <c r="H48"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>88</v>
       </c>
@@ -2737,7 +2744,7 @@
       </c>
       <c r="H49"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>88</v>
       </c>
@@ -2758,7 +2765,7 @@
       </c>
       <c r="H50"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>88</v>
       </c>
@@ -2779,7 +2786,7 @@
       </c>
       <c r="H51"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>88</v>
       </c>
@@ -2800,7 +2807,7 @@
       </c>
       <c r="H52"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>109</v>
       </c>
@@ -2821,7 +2828,7 @@
       </c>
       <c r="H53"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>109</v>
       </c>
@@ -2842,7 +2849,7 @@
       </c>
       <c r="H54"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>109</v>
       </c>
@@ -2863,7 +2870,7 @@
       </c>
       <c r="H55"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>109</v>
       </c>
@@ -2884,7 +2891,7 @@
       </c>
       <c r="H56"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>109</v>
       </c>
@@ -2905,7 +2912,7 @@
       </c>
       <c r="H57"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>109</v>
       </c>
@@ -2926,7 +2933,7 @@
       </c>
       <c r="H58"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>109</v>
       </c>
@@ -2947,7 +2954,7 @@
       </c>
       <c r="H59"/>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>109</v>
       </c>
@@ -2968,7 +2975,7 @@
       </c>
       <c r="H60"/>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>56</v>
       </c>
@@ -2989,7 +2996,7 @@
       </c>
       <c r="H61"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>56</v>
       </c>
@@ -3010,7 +3017,7 @@
       </c>
       <c r="H62"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>56</v>
       </c>
@@ -3031,7 +3038,7 @@
       </c>
       <c r="H63"/>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>56</v>
       </c>
@@ -3052,7 +3059,7 @@
       </c>
       <c r="H64"/>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>56</v>
       </c>
@@ -3073,7 +3080,7 @@
       </c>
       <c r="H65"/>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>56</v>
       </c>
@@ -3094,7 +3101,7 @@
       </c>
       <c r="H66"/>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>56</v>
       </c>
@@ -3115,7 +3122,7 @@
       </c>
       <c r="H67"/>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>56</v>
       </c>
@@ -3136,7 +3143,7 @@
       </c>
       <c r="H68"/>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>56</v>
       </c>
@@ -3157,7 +3164,7 @@
       </c>
       <c r="H69"/>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>56</v>
       </c>
@@ -3178,7 +3185,7 @@
       </c>
       <c r="H70"/>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>56</v>
       </c>
@@ -3199,7 +3206,7 @@
       </c>
       <c r="H71"/>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>56</v>
       </c>
@@ -3220,7 +3227,7 @@
       </c>
       <c r="H72"/>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>56</v>
       </c>
@@ -3241,7 +3248,7 @@
       </c>
       <c r="H73"/>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>56</v>
       </c>
@@ -3262,7 +3269,7 @@
       </c>
       <c r="H74"/>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>56</v>
       </c>
@@ -3283,7 +3290,7 @@
       </c>
       <c r="H75"/>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>56</v>
       </c>
@@ -3304,7 +3311,7 @@
       </c>
       <c r="H76"/>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>56</v>
       </c>
@@ -3325,7 +3332,7 @@
       </c>
       <c r="H77"/>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>56</v>
       </c>
@@ -3346,7 +3353,7 @@
       </c>
       <c r="H78"/>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>162</v>
       </c>
@@ -3367,7 +3374,7 @@
       </c>
       <c r="H79"/>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>162</v>
       </c>
@@ -3388,7 +3395,7 @@
       </c>
       <c r="H80"/>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>162</v>
       </c>
@@ -3409,7 +3416,7 @@
       </c>
       <c r="H81"/>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>162</v>
       </c>
@@ -3430,7 +3437,7 @@
       </c>
       <c r="H82"/>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>162</v>
       </c>
@@ -3451,7 +3458,7 @@
       </c>
       <c r="H83"/>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>162</v>
       </c>
@@ -3472,7 +3479,7 @@
       </c>
       <c r="H84"/>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>162</v>
       </c>
@@ -3493,7 +3500,7 @@
       </c>
       <c r="H85"/>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>177</v>
       </c>
@@ -3514,7 +3521,7 @@
       </c>
       <c r="H86"/>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>177</v>
       </c>
@@ -3535,7 +3542,7 @@
       </c>
       <c r="H87"/>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>177</v>
       </c>
@@ -3556,7 +3563,7 @@
       </c>
       <c r="H88"/>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>177</v>
       </c>
@@ -3577,7 +3584,7 @@
       </c>
       <c r="H89"/>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>177</v>
       </c>
@@ -3598,7 +3605,7 @@
       </c>
       <c r="H90"/>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>177</v>
       </c>
@@ -3619,7 +3626,7 @@
       </c>
       <c r="H91"/>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>177</v>
       </c>
@@ -3640,7 +3647,7 @@
       </c>
       <c r="H92"/>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>177</v>
       </c>
@@ -3661,7 +3668,7 @@
       </c>
       <c r="H93"/>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>177</v>
       </c>
@@ -3682,7 +3689,7 @@
       </c>
       <c r="H94"/>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>177</v>
       </c>
@@ -3703,7 +3710,7 @@
       </c>
       <c r="H95"/>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>177</v>
       </c>
@@ -3724,7 +3731,7 @@
       </c>
       <c r="H96"/>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>177</v>
       </c>
@@ -3745,7 +3752,7 @@
       </c>
       <c r="H97"/>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>177</v>
       </c>
@@ -3766,7 +3773,7 @@
       </c>
       <c r="H98"/>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>177</v>
       </c>
@@ -3787,7 +3794,7 @@
       </c>
       <c r="H99"/>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>177</v>
       </c>
@@ -3808,7 +3815,7 @@
       </c>
       <c r="H100"/>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>177</v>
       </c>
@@ -3829,7 +3836,7 @@
       </c>
       <c r="H101"/>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>177</v>
       </c>
@@ -3850,7 +3857,7 @@
       </c>
       <c r="H102"/>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>177</v>
       </c>
@@ -3871,7 +3878,7 @@
       </c>
       <c r="H103"/>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>177</v>
       </c>
@@ -3892,7 +3899,7 @@
       </c>
       <c r="H104"/>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>177</v>
       </c>
@@ -3913,7 +3920,7 @@
       </c>
       <c r="H105"/>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>177</v>
       </c>
@@ -3960,7 +3967,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>222</v>
       </c>
@@ -3981,7 +3988,7 @@
       </c>
       <c r="H108"/>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>222</v>
       </c>
@@ -4002,7 +4009,7 @@
       </c>
       <c r="H109"/>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>222</v>
       </c>
@@ -4023,7 +4030,7 @@
       </c>
       <c r="H110"/>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>222</v>
       </c>
@@ -4044,7 +4051,7 @@
       </c>
       <c r="H111"/>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>222</v>
       </c>
@@ -4065,7 +4072,7 @@
       </c>
       <c r="H112"/>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>222</v>
       </c>
@@ -4086,7 +4093,7 @@
       </c>
       <c r="H113"/>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>177</v>
       </c>
@@ -4107,7 +4114,7 @@
       </c>
       <c r="H114"/>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>237</v>
       </c>
@@ -4128,7 +4135,7 @@
       </c>
       <c r="H115"/>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>237</v>
       </c>
@@ -4149,7 +4156,7 @@
       </c>
       <c r="H116"/>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>237</v>
       </c>
@@ -4170,7 +4177,7 @@
       </c>
       <c r="H117"/>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>244</v>
       </c>
@@ -4191,7 +4198,7 @@
       </c>
       <c r="H118"/>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>244</v>
       </c>
@@ -4212,7 +4219,7 @@
       </c>
       <c r="H119"/>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>244</v>
       </c>
@@ -4233,7 +4240,7 @@
       </c>
       <c r="H120"/>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>244</v>
       </c>
@@ -4254,7 +4261,7 @@
       </c>
       <c r="H121"/>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>3</v>
       </c>
@@ -4275,7 +4282,7 @@
       </c>
       <c r="H122"/>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>3</v>
       </c>
@@ -4296,7 +4303,7 @@
       </c>
       <c r="H123"/>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>3</v>
       </c>
@@ -4317,7 +4324,7 @@
       </c>
       <c r="H124"/>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>3</v>
       </c>
@@ -4338,7 +4345,7 @@
       </c>
       <c r="H125"/>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>3</v>
       </c>
@@ -4359,7 +4366,7 @@
       </c>
       <c r="H126"/>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>3</v>
       </c>
@@ -4380,7 +4387,7 @@
       </c>
       <c r="H127"/>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>3</v>
       </c>
@@ -4401,7 +4408,7 @@
       </c>
       <c r="H128"/>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>3</v>
       </c>
@@ -4422,7 +4429,7 @@
       </c>
       <c r="H129"/>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>3</v>
       </c>
@@ -4443,7 +4450,7 @@
       </c>
       <c r="H130"/>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>3</v>
       </c>
@@ -4464,7 +4471,7 @@
       </c>
       <c r="H131"/>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>162</v>
       </c>
@@ -4485,7 +4492,7 @@
       </c>
       <c r="H132"/>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>162</v>
       </c>
@@ -4506,7 +4513,7 @@
       </c>
       <c r="H133"/>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>109</v>
       </c>
@@ -4527,7 +4534,7 @@
       </c>
       <c r="H134"/>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>109</v>
       </c>
@@ -4548,7 +4555,7 @@
       </c>
       <c r="H135"/>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>56</v>
       </c>
@@ -4569,7 +4576,7 @@
       </c>
       <c r="H136"/>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>56</v>
       </c>
@@ -4590,7 +4597,7 @@
       </c>
       <c r="H137"/>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>162</v>
       </c>
@@ -4611,7 +4618,7 @@
       </c>
       <c r="H138"/>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>177</v>
       </c>
@@ -4632,7 +4639,7 @@
       </c>
       <c r="H139"/>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>3</v>
       </c>
@@ -4653,7 +4660,7 @@
       </c>
       <c r="H140"/>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>3</v>
       </c>
@@ -4674,7 +4681,7 @@
       </c>
       <c r="H141"/>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>65</v>
       </c>
@@ -4695,8 +4702,26 @@
       </c>
       <c r="H142"/>
     </row>
+    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C143" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C144" t="s">
+        <v>442</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:G142"/>
+  <autoFilter ref="A1:G142">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="Cervical cancer (first line)"/>
+        <filter val="Cervical cancer screening"/>
+        <filter val="HPV vaccine"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <conditionalFormatting sqref="F1:F1048576 G11">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Updates to Xpert test
-Remove full untargeted expert since this intervention is treated as incremental to 104-106

-remove from list of substitutes

-for the targeted intervention, use Targeted-Xpert-MDR-HIV-FN-Spot-Spot from Tesfaye instead of Targeted-Xpert-ZN-Negative-Spot-Morning-Spot since this is the most cost-effective version
</commit_message>
<xml_diff>
--- a/2_data/new_intervention_names.xlsx
+++ b/2_data/new_intervention_names.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$142</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$144</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="443">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="447">
   <si>
     <t>Category</t>
   </si>
@@ -1289,9 +1289,6 @@
     <t>Isoniazid Preventive Therapy for children in contact with TB patients</t>
   </si>
   <si>
-    <t>Full DOTS (smear-positive, smear negative and extrapulmonary cases)</t>
-  </si>
-  <si>
     <t>Mass media campaigns for HIV prevention</t>
   </si>
   <si>
@@ -1352,10 +1349,25 @@
     <t>Basic psychosocial support, advice, and follow-up (including antidepressants)</t>
   </si>
   <si>
-    <t>Smear test at age 40 fo cervical cancer detection + cancer treatment</t>
-  </si>
-  <si>
-    <t>Smear test at age 40 fo cervical cancer detection + HPV vaccinations starting at age 12 + cancer treatment</t>
+    <t>Smear test at age 40 for cervical cancer detection + cancer treatment</t>
+  </si>
+  <si>
+    <t>Smear test at age 40 for cervical cancer detection + HPV vaccinations starting at age 12 + cancer treatment</t>
+  </si>
+  <si>
+    <t>Xpert test (All presumptive TB cases)</t>
+  </si>
+  <si>
+    <t>Xpert test (Specific cases - HIV +ve, known contact of MDR-TB cases, retreatment cases)</t>
+  </si>
+  <si>
+    <t>Minimal DOTS (smear positive cases)</t>
+  </si>
+  <si>
+    <t>Full DOTS (smear negative and extrapulmonary cases)</t>
+  </si>
+  <si>
+    <t>Full combination DOTS  (MDR cases)</t>
   </si>
 </sst>
 </file>
@@ -1392,7 +1404,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -1400,17 +1412,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1703,11 +1731,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:I144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F145" sqref="F145"/>
+    <sheetView tabSelected="1" topLeftCell="B118" workbookViewId="0">
+      <selection activeCell="D135" sqref="D135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1739,7 +1766,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1760,7 +1787,7 @@
       </c>
       <c r="H2"/>
     </row>
-    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1781,7 +1808,7 @@
       </c>
       <c r="H3"/>
     </row>
-    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1802,7 +1829,7 @@
       </c>
       <c r="H4"/>
     </row>
-    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1823,7 +1850,7 @@
       </c>
       <c r="H5"/>
     </row>
-    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -1844,7 +1871,7 @@
       </c>
       <c r="H6"/>
     </row>
-    <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -1865,7 +1892,7 @@
       </c>
       <c r="H7"/>
     </row>
-    <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -1886,7 +1913,7 @@
       </c>
       <c r="H8"/>
     </row>
-    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -1907,7 +1934,7 @@
       </c>
       <c r="H9"/>
     </row>
-    <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -1928,7 +1955,7 @@
       </c>
       <c r="H10"/>
     </row>
-    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -1952,7 +1979,7 @@
       </c>
       <c r="H11"/>
     </row>
-    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -1973,7 +2000,7 @@
       </c>
       <c r="H12"/>
     </row>
-    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -1994,7 +2021,7 @@
       </c>
       <c r="H13"/>
     </row>
-    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -2015,7 +2042,7 @@
       </c>
       <c r="H14"/>
     </row>
-    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -2036,7 +2063,7 @@
       </c>
       <c r="H15"/>
     </row>
-    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -2057,7 +2084,7 @@
       </c>
       <c r="H16"/>
     </row>
-    <row r="17" spans="1:6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>3</v>
       </c>
@@ -2077,7 +2104,7 @@
         <v>12.287983160102591</v>
       </c>
     </row>
-    <row r="18" spans="1:6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>3</v>
       </c>
@@ -2097,7 +2124,7 @@
         <v>5.8764426199980653</v>
       </c>
     </row>
-    <row r="19" spans="1:6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>3</v>
       </c>
@@ -2117,7 +2144,7 @@
         <v>22.626927498876491</v>
       </c>
     </row>
-    <row r="20" spans="1:6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>3</v>
       </c>
@@ -2137,7 +2164,7 @@
         <v>22.626927498876483</v>
       </c>
     </row>
-    <row r="21" spans="1:6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>3</v>
       </c>
@@ -2157,7 +2184,7 @@
         <v>4.810820102639263</v>
       </c>
     </row>
-    <row r="22" spans="1:6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>3</v>
       </c>
@@ -2177,7 +2204,7 @@
         <v>43.937776702649238</v>
       </c>
     </row>
-    <row r="23" spans="1:6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>3</v>
       </c>
@@ -2197,7 +2224,7 @@
         <v>69.987315823932676</v>
       </c>
     </row>
-    <row r="24" spans="1:6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>3</v>
       </c>
@@ -2217,7 +2244,7 @@
         <v>3.0761982466467503</v>
       </c>
     </row>
-    <row r="25" spans="1:6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>3</v>
       </c>
@@ -2237,7 +2264,7 @@
         <v>68.864561953102353</v>
       </c>
     </row>
-    <row r="26" spans="1:6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>3</v>
       </c>
@@ -2257,7 +2284,7 @@
         <v>36.727766374987922</v>
       </c>
     </row>
-    <row r="27" spans="1:6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>3</v>
       </c>
@@ -2277,7 +2304,7 @@
         <v>19.248450535311211</v>
       </c>
     </row>
-    <row r="28" spans="1:6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>56</v>
       </c>
@@ -2297,7 +2324,7 @@
         <v>17.768996830715984</v>
       </c>
     </row>
-    <row r="29" spans="1:6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>56</v>
       </c>
@@ -2317,7 +2344,7 @@
         <v>17.768996830715984</v>
       </c>
     </row>
-    <row r="30" spans="1:6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>56</v>
       </c>
@@ -2337,7 +2364,7 @@
         <v>17.768996830715984</v>
       </c>
     </row>
-    <row r="31" spans="1:6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>56</v>
       </c>
@@ -2357,7 +2384,7 @@
         <v>17.768996830715988</v>
       </c>
     </row>
-    <row r="32" spans="1:6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>65</v>
       </c>
@@ -2377,7 +2404,7 @@
         <v>60.706723287675047</v>
       </c>
     </row>
-    <row r="33" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>65</v>
       </c>
@@ -2398,7 +2425,7 @@
       </c>
       <c r="H33"/>
     </row>
-    <row r="34" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>65</v>
       </c>
@@ -2419,7 +2446,7 @@
       </c>
       <c r="H34"/>
     </row>
-    <row r="35" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>65</v>
       </c>
@@ -2440,7 +2467,7 @@
       </c>
       <c r="H35"/>
     </row>
-    <row r="36" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>65</v>
       </c>
@@ -2461,7 +2488,7 @@
       </c>
       <c r="H36"/>
     </row>
-    <row r="37" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>65</v>
       </c>
@@ -2482,7 +2509,7 @@
       </c>
       <c r="H37"/>
     </row>
-    <row r="38" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>65</v>
       </c>
@@ -2503,7 +2530,7 @@
       </c>
       <c r="H38"/>
     </row>
-    <row r="39" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>65</v>
       </c>
@@ -2576,7 +2603,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="42" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>65</v>
       </c>
@@ -2597,7 +2624,7 @@
       </c>
       <c r="H42"/>
     </row>
-    <row r="43" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>88</v>
       </c>
@@ -2618,7 +2645,7 @@
       </c>
       <c r="H43"/>
     </row>
-    <row r="44" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>88</v>
       </c>
@@ -2639,7 +2666,7 @@
       </c>
       <c r="H44"/>
     </row>
-    <row r="45" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>88</v>
       </c>
@@ -2660,7 +2687,7 @@
       </c>
       <c r="H45"/>
     </row>
-    <row r="46" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>88</v>
       </c>
@@ -2681,7 +2708,7 @@
       </c>
       <c r="H46"/>
     </row>
-    <row r="47" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>88</v>
       </c>
@@ -2702,7 +2729,7 @@
       </c>
       <c r="H47"/>
     </row>
-    <row r="48" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>88</v>
       </c>
@@ -2723,7 +2750,7 @@
       </c>
       <c r="H48"/>
     </row>
-    <row r="49" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>88</v>
       </c>
@@ -2744,7 +2771,7 @@
       </c>
       <c r="H49"/>
     </row>
-    <row r="50" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>88</v>
       </c>
@@ -2765,7 +2792,7 @@
       </c>
       <c r="H50"/>
     </row>
-    <row r="51" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>88</v>
       </c>
@@ -2786,7 +2813,7 @@
       </c>
       <c r="H51"/>
     </row>
-    <row r="52" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>88</v>
       </c>
@@ -2807,7 +2834,7 @@
       </c>
       <c r="H52"/>
     </row>
-    <row r="53" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>109</v>
       </c>
@@ -2828,7 +2855,7 @@
       </c>
       <c r="H53"/>
     </row>
-    <row r="54" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>109</v>
       </c>
@@ -2849,7 +2876,7 @@
       </c>
       <c r="H54"/>
     </row>
-    <row r="55" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>109</v>
       </c>
@@ -2870,7 +2897,7 @@
       </c>
       <c r="H55"/>
     </row>
-    <row r="56" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>109</v>
       </c>
@@ -2878,7 +2905,7 @@
         <v>116</v>
       </c>
       <c r="C56" t="s">
-        <v>117</v>
+        <v>444</v>
       </c>
       <c r="D56" t="s">
         <v>117</v>
@@ -2891,7 +2918,7 @@
       </c>
       <c r="H56"/>
     </row>
-    <row r="57" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>109</v>
       </c>
@@ -2899,7 +2926,7 @@
         <v>118</v>
       </c>
       <c r="C57" t="s">
-        <v>420</v>
+        <v>445</v>
       </c>
       <c r="D57" t="s">
         <v>119</v>
@@ -2912,7 +2939,7 @@
       </c>
       <c r="H57"/>
     </row>
-    <row r="58" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>109</v>
       </c>
@@ -2920,7 +2947,7 @@
         <v>120</v>
       </c>
       <c r="C58" t="s">
-        <v>121</v>
+        <v>446</v>
       </c>
       <c r="D58" t="s">
         <v>121</v>
@@ -2933,7 +2960,7 @@
       </c>
       <c r="H58"/>
     </row>
-    <row r="59" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>109</v>
       </c>
@@ -2954,7 +2981,7 @@
       </c>
       <c r="H59"/>
     </row>
-    <row r="60" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>109</v>
       </c>
@@ -2975,7 +3002,7 @@
       </c>
       <c r="H60"/>
     </row>
-    <row r="61" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>56</v>
       </c>
@@ -2996,7 +3023,7 @@
       </c>
       <c r="H61"/>
     </row>
-    <row r="62" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>56</v>
       </c>
@@ -3004,7 +3031,7 @@
         <v>128</v>
       </c>
       <c r="C62" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D62" t="s">
         <v>129</v>
@@ -3017,7 +3044,7 @@
       </c>
       <c r="H62"/>
     </row>
-    <row r="63" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>56</v>
       </c>
@@ -3025,7 +3052,7 @@
         <v>130</v>
       </c>
       <c r="C63" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D63" t="s">
         <v>131</v>
@@ -3038,7 +3065,7 @@
       </c>
       <c r="H63"/>
     </row>
-    <row r="64" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>56</v>
       </c>
@@ -3046,7 +3073,7 @@
         <v>132</v>
       </c>
       <c r="C64" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D64" t="s">
         <v>133</v>
@@ -3059,7 +3086,7 @@
       </c>
       <c r="H64"/>
     </row>
-    <row r="65" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>56</v>
       </c>
@@ -3080,7 +3107,7 @@
       </c>
       <c r="H65"/>
     </row>
-    <row r="66" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>56</v>
       </c>
@@ -3101,7 +3128,7 @@
       </c>
       <c r="H66"/>
     </row>
-    <row r="67" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>56</v>
       </c>
@@ -3122,7 +3149,7 @@
       </c>
       <c r="H67"/>
     </row>
-    <row r="68" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>56</v>
       </c>
@@ -3143,7 +3170,7 @@
       </c>
       <c r="H68"/>
     </row>
-    <row r="69" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>56</v>
       </c>
@@ -3151,7 +3178,7 @@
         <v>142</v>
       </c>
       <c r="C69" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D69" t="s">
         <v>143</v>
@@ -3164,7 +3191,7 @@
       </c>
       <c r="H69"/>
     </row>
-    <row r="70" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>56</v>
       </c>
@@ -3172,7 +3199,7 @@
         <v>144</v>
       </c>
       <c r="C70" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="D70" t="s">
         <v>145</v>
@@ -3185,7 +3212,7 @@
       </c>
       <c r="H70"/>
     </row>
-    <row r="71" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>56</v>
       </c>
@@ -3206,7 +3233,7 @@
       </c>
       <c r="H71"/>
     </row>
-    <row r="72" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>56</v>
       </c>
@@ -3214,7 +3241,7 @@
         <v>148</v>
       </c>
       <c r="C72" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D72" t="s">
         <v>149</v>
@@ -3227,7 +3254,7 @@
       </c>
       <c r="H72"/>
     </row>
-    <row r="73" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>56</v>
       </c>
@@ -3248,7 +3275,7 @@
       </c>
       <c r="H73"/>
     </row>
-    <row r="74" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>56</v>
       </c>
@@ -3269,7 +3296,7 @@
       </c>
       <c r="H74"/>
     </row>
-    <row r="75" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>56</v>
       </c>
@@ -3277,7 +3304,7 @@
         <v>154</v>
       </c>
       <c r="C75" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D75" t="s">
         <v>155</v>
@@ -3290,7 +3317,7 @@
       </c>
       <c r="H75"/>
     </row>
-    <row r="76" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>56</v>
       </c>
@@ -3298,7 +3325,7 @@
         <v>156</v>
       </c>
       <c r="C76" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="D76" t="s">
         <v>157</v>
@@ -3311,7 +3338,7 @@
       </c>
       <c r="H76"/>
     </row>
-    <row r="77" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>56</v>
       </c>
@@ -3332,7 +3359,7 @@
       </c>
       <c r="H77"/>
     </row>
-    <row r="78" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>56</v>
       </c>
@@ -3340,7 +3367,7 @@
         <v>160</v>
       </c>
       <c r="C78" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="D78" t="s">
         <v>161</v>
@@ -3353,7 +3380,7 @@
       </c>
       <c r="H78"/>
     </row>
-    <row r="79" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>162</v>
       </c>
@@ -3361,7 +3388,7 @@
         <v>163</v>
       </c>
       <c r="C79" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D79" t="s">
         <v>164</v>
@@ -3374,7 +3401,7 @@
       </c>
       <c r="H79"/>
     </row>
-    <row r="80" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>162</v>
       </c>
@@ -3395,7 +3422,7 @@
       </c>
       <c r="H80"/>
     </row>
-    <row r="81" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>162</v>
       </c>
@@ -3403,7 +3430,7 @@
         <v>167</v>
       </c>
       <c r="C81" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D81" t="s">
         <v>168</v>
@@ -3416,7 +3443,7 @@
       </c>
       <c r="H81"/>
     </row>
-    <row r="82" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>162</v>
       </c>
@@ -3437,7 +3464,7 @@
       </c>
       <c r="H82"/>
     </row>
-    <row r="83" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>162</v>
       </c>
@@ -3458,7 +3485,7 @@
       </c>
       <c r="H83"/>
     </row>
-    <row r="84" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>162</v>
       </c>
@@ -3479,7 +3506,7 @@
       </c>
       <c r="H84"/>
     </row>
-    <row r="85" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>162</v>
       </c>
@@ -3500,7 +3527,7 @@
       </c>
       <c r="H85"/>
     </row>
-    <row r="86" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>177</v>
       </c>
@@ -3521,7 +3548,7 @@
       </c>
       <c r="H86"/>
     </row>
-    <row r="87" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>177</v>
       </c>
@@ -3529,7 +3556,7 @@
         <v>180</v>
       </c>
       <c r="C87" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="D87" t="s">
         <v>181</v>
@@ -3542,7 +3569,7 @@
       </c>
       <c r="H87"/>
     </row>
-    <row r="88" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>177</v>
       </c>
@@ -3563,7 +3590,7 @@
       </c>
       <c r="H88"/>
     </row>
-    <row r="89" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>177</v>
       </c>
@@ -3584,7 +3611,7 @@
       </c>
       <c r="H89"/>
     </row>
-    <row r="90" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>177</v>
       </c>
@@ -3605,7 +3632,7 @@
       </c>
       <c r="H90"/>
     </row>
-    <row r="91" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>177</v>
       </c>
@@ -3626,7 +3653,7 @@
       </c>
       <c r="H91"/>
     </row>
-    <row r="92" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>177</v>
       </c>
@@ -3647,7 +3674,7 @@
       </c>
       <c r="H92"/>
     </row>
-    <row r="93" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>177</v>
       </c>
@@ -3668,7 +3695,7 @@
       </c>
       <c r="H93"/>
     </row>
-    <row r="94" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>177</v>
       </c>
@@ -3689,7 +3716,7 @@
       </c>
       <c r="H94"/>
     </row>
-    <row r="95" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>177</v>
       </c>
@@ -3710,7 +3737,7 @@
       </c>
       <c r="H95"/>
     </row>
-    <row r="96" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>177</v>
       </c>
@@ -3731,7 +3758,7 @@
       </c>
       <c r="H96"/>
     </row>
-    <row r="97" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>177</v>
       </c>
@@ -3752,7 +3779,7 @@
       </c>
       <c r="H97"/>
     </row>
-    <row r="98" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>177</v>
       </c>
@@ -3773,7 +3800,7 @@
       </c>
       <c r="H98"/>
     </row>
-    <row r="99" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>177</v>
       </c>
@@ -3781,7 +3808,7 @@
         <v>204</v>
       </c>
       <c r="C99" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D99" t="s">
         <v>205</v>
@@ -3794,7 +3821,7 @@
       </c>
       <c r="H99"/>
     </row>
-    <row r="100" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>177</v>
       </c>
@@ -3802,7 +3829,7 @@
         <v>206</v>
       </c>
       <c r="C100" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D100" t="s">
         <v>207</v>
@@ -3815,7 +3842,7 @@
       </c>
       <c r="H100"/>
     </row>
-    <row r="101" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>177</v>
       </c>
@@ -3836,7 +3863,7 @@
       </c>
       <c r="H101"/>
     </row>
-    <row r="102" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>177</v>
       </c>
@@ -3857,7 +3884,7 @@
       </c>
       <c r="H102"/>
     </row>
-    <row r="103" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>177</v>
       </c>
@@ -3878,7 +3905,7 @@
       </c>
       <c r="H103"/>
     </row>
-    <row r="104" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>177</v>
       </c>
@@ -3886,7 +3913,7 @@
         <v>214</v>
       </c>
       <c r="C104" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D104" t="s">
         <v>215</v>
@@ -3899,7 +3926,7 @@
       </c>
       <c r="H104"/>
     </row>
-    <row r="105" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>177</v>
       </c>
@@ -3920,7 +3947,7 @@
       </c>
       <c r="H105"/>
     </row>
-    <row r="106" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>177</v>
       </c>
@@ -3928,7 +3955,7 @@
         <v>218</v>
       </c>
       <c r="C106" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D106" t="s">
         <v>219</v>
@@ -3967,7 +3994,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="108" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>222</v>
       </c>
@@ -3975,7 +4002,7 @@
         <v>223</v>
       </c>
       <c r="C108" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="D108" t="s">
         <v>224</v>
@@ -3988,7 +4015,7 @@
       </c>
       <c r="H108"/>
     </row>
-    <row r="109" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>222</v>
       </c>
@@ -3996,7 +4023,7 @@
         <v>225</v>
       </c>
       <c r="C109" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D109" t="s">
         <v>226</v>
@@ -4009,7 +4036,7 @@
       </c>
       <c r="H109"/>
     </row>
-    <row r="110" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>222</v>
       </c>
@@ -4017,7 +4044,7 @@
         <v>227</v>
       </c>
       <c r="C110" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="D110" t="s">
         <v>228</v>
@@ -4030,7 +4057,7 @@
       </c>
       <c r="H110"/>
     </row>
-    <row r="111" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>222</v>
       </c>
@@ -4051,7 +4078,7 @@
       </c>
       <c r="H111"/>
     </row>
-    <row r="112" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>222</v>
       </c>
@@ -4059,7 +4086,7 @@
         <v>231</v>
       </c>
       <c r="C112" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D112" t="s">
         <v>232</v>
@@ -4072,7 +4099,7 @@
       </c>
       <c r="H112"/>
     </row>
-    <row r="113" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>222</v>
       </c>
@@ -4093,7 +4120,7 @@
       </c>
       <c r="H113"/>
     </row>
-    <row r="114" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>177</v>
       </c>
@@ -4114,7 +4141,7 @@
       </c>
       <c r="H114"/>
     </row>
-    <row r="115" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>237</v>
       </c>
@@ -4135,7 +4162,7 @@
       </c>
       <c r="H115"/>
     </row>
-    <row r="116" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>237</v>
       </c>
@@ -4156,7 +4183,7 @@
       </c>
       <c r="H116"/>
     </row>
-    <row r="117" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>237</v>
       </c>
@@ -4177,7 +4204,7 @@
       </c>
       <c r="H117"/>
     </row>
-    <row r="118" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>244</v>
       </c>
@@ -4198,7 +4225,7 @@
       </c>
       <c r="H118"/>
     </row>
-    <row r="119" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>244</v>
       </c>
@@ -4219,7 +4246,7 @@
       </c>
       <c r="H119"/>
     </row>
-    <row r="120" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>244</v>
       </c>
@@ -4240,7 +4267,7 @@
       </c>
       <c r="H120"/>
     </row>
-    <row r="121" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>244</v>
       </c>
@@ -4261,7 +4288,7 @@
       </c>
       <c r="H121"/>
     </row>
-    <row r="122" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>3</v>
       </c>
@@ -4282,7 +4309,7 @@
       </c>
       <c r="H122"/>
     </row>
-    <row r="123" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>3</v>
       </c>
@@ -4303,7 +4330,7 @@
       </c>
       <c r="H123"/>
     </row>
-    <row r="124" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>3</v>
       </c>
@@ -4324,7 +4351,7 @@
       </c>
       <c r="H124"/>
     </row>
-    <row r="125" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>3</v>
       </c>
@@ -4345,7 +4372,7 @@
       </c>
       <c r="H125"/>
     </row>
-    <row r="126" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>3</v>
       </c>
@@ -4366,7 +4393,7 @@
       </c>
       <c r="H126"/>
     </row>
-    <row r="127" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>3</v>
       </c>
@@ -4387,7 +4414,7 @@
       </c>
       <c r="H127"/>
     </row>
-    <row r="128" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>3</v>
       </c>
@@ -4408,7 +4435,7 @@
       </c>
       <c r="H128"/>
     </row>
-    <row r="129" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>3</v>
       </c>
@@ -4429,7 +4456,7 @@
       </c>
       <c r="H129"/>
     </row>
-    <row r="130" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>3</v>
       </c>
@@ -4450,7 +4477,7 @@
       </c>
       <c r="H130"/>
     </row>
-    <row r="131" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>3</v>
       </c>
@@ -4471,7 +4498,7 @@
       </c>
       <c r="H131"/>
     </row>
-    <row r="132" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>162</v>
       </c>
@@ -4492,7 +4519,7 @@
       </c>
       <c r="H132"/>
     </row>
-    <row r="133" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>162</v>
       </c>
@@ -4513,7 +4540,7 @@
       </c>
       <c r="H133"/>
     </row>
-    <row r="134" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>109</v>
       </c>
@@ -4521,7 +4548,7 @@
         <v>277</v>
       </c>
       <c r="C134" t="s">
-        <v>278</v>
+        <v>442</v>
       </c>
       <c r="D134" t="s">
         <v>278</v>
@@ -4534,7 +4561,7 @@
       </c>
       <c r="H134"/>
     </row>
-    <row r="135" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>109</v>
       </c>
@@ -4542,7 +4569,7 @@
         <v>279</v>
       </c>
       <c r="C135" t="s">
-        <v>280</v>
+        <v>443</v>
       </c>
       <c r="D135" t="s">
         <v>280</v>
@@ -4555,7 +4582,7 @@
       </c>
       <c r="H135"/>
     </row>
-    <row r="136" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>56</v>
       </c>
@@ -4576,7 +4603,7 @@
       </c>
       <c r="H136"/>
     </row>
-    <row r="137" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>56</v>
       </c>
@@ -4597,7 +4624,7 @@
       </c>
       <c r="H137"/>
     </row>
-    <row r="138" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>162</v>
       </c>
@@ -4618,7 +4645,7 @@
       </c>
       <c r="H138"/>
     </row>
-    <row r="139" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>177</v>
       </c>
@@ -4639,7 +4666,7 @@
       </c>
       <c r="H139"/>
     </row>
-    <row r="140" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>3</v>
       </c>
@@ -4660,7 +4687,7 @@
       </c>
       <c r="H140"/>
     </row>
-    <row r="141" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>3</v>
       </c>
@@ -4681,7 +4708,7 @@
       </c>
       <c r="H141"/>
     </row>
-    <row r="142" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>65</v>
       </c>
@@ -4703,25 +4730,29 @@
       <c r="H142"/>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C143" t="s">
+      <c r="B143">
+        <v>350</v>
+      </c>
+      <c r="C143" s="3" t="s">
+        <v>440</v>
+      </c>
+      <c r="D143" s="3" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B144">
+        <v>351</v>
+      </c>
+      <c r="C144" s="3" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C144" t="s">
-        <v>442</v>
+      <c r="D144" s="3" t="s">
+        <v>441</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G142">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="Cervical cancer (first line)"/>
-        <filter val="Cervical cancer screening"/>
-        <filter val="HPV vaccine"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:G144"/>
   <conditionalFormatting sqref="F1:F1048576 G11">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>

</xml_diff>

<commit_message>
update name of intervention - vaginal delivery
</commit_message>
<xml_diff>
--- a/2_data/new_intervention_names.xlsx
+++ b/2_data/new_intervention_names.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="717" uniqueCount="445">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="447">
   <si>
     <t>Category</t>
   </si>
@@ -1362,6 +1362,12 @@
   </si>
   <si>
     <t>Vaginal Delivery without complication (skilled attendance)</t>
+  </si>
+  <si>
+    <t>Vaginal delivery without complication - skilled attendance (including active management of third stage of labour)</t>
+  </si>
+  <si>
+    <t>Vaginal Delivery with complication (including active management of third stage of labour)</t>
   </si>
 </sst>
 </file>
@@ -1726,10 +1732,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H144"/>
+  <dimension ref="A1:H147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="B76" workbookViewId="0">
+      <selection activeCell="C93" sqref="C93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4883,7 +4889,7 @@
         <v>119.10574499199393</v>
       </c>
       <c r="H131" t="b">
-        <f t="shared" ref="H131:H144" si="2">D131=C131</f>
+        <f t="shared" ref="H131:H147" si="2">D131=C131</f>
         <v>1</v>
       </c>
     </row>
@@ -5179,6 +5185,36 @@
       <c r="H144" t="b">
         <f t="shared" si="2"/>
         <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H145" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B146">
+        <v>353</v>
+      </c>
+      <c r="C146" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="H146" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B147">
+        <v>354</v>
+      </c>
+      <c r="C147" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="H147" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changes names of contraception interventions
</commit_message>
<xml_diff>
--- a/2_data/new_intervention_names.xlsx
+++ b/2_data/new_intervention_names.xlsx
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$144</definedName>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="447">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="455">
   <si>
     <t>Category</t>
   </si>
@@ -1368,6 +1369,30 @@
   </si>
   <si>
     <t>Vaginal Delivery with complication (including active management of third stage of labour)</t>
+  </si>
+  <si>
+    <t>Modern contraceptive: Condoms</t>
+  </si>
+  <si>
+    <t>Modern contraceptive: Female condoms</t>
+  </si>
+  <si>
+    <t>Modern contraceptive: Oral contraceptive pill</t>
+  </si>
+  <si>
+    <t>Modern contraception: Long-acting injectable hormones</t>
+  </si>
+  <si>
+    <t>Modern contraception: Intrauterine device (IUD)</t>
+  </si>
+  <si>
+    <t>Modern contraception: Levonorgestrel-releasing implant</t>
+  </si>
+  <si>
+    <t>Modern contraception: Female sterilization</t>
+  </si>
+  <si>
+    <t>Modern contraception: Male sterilization</t>
   </si>
 </sst>
 </file>
@@ -1734,8 +1759,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B76" workbookViewId="0">
-      <selection activeCell="C93" sqref="C93"/>
+    <sheetView tabSelected="1" topLeftCell="B115" workbookViewId="0">
+      <selection activeCell="C127" sqref="C127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4661,7 +4686,7 @@
         <v>253</v>
       </c>
       <c r="C122" t="s">
-        <v>254</v>
+        <v>449</v>
       </c>
       <c r="D122" t="s">
         <v>254</v>
@@ -4674,7 +4699,7 @@
       </c>
       <c r="H122" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.25">
@@ -4685,7 +4710,7 @@
         <v>255</v>
       </c>
       <c r="C123" t="s">
-        <v>256</v>
+        <v>447</v>
       </c>
       <c r="D123" t="s">
         <v>256</v>
@@ -4698,7 +4723,7 @@
       </c>
       <c r="H123" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.25">
@@ -4709,7 +4734,7 @@
         <v>257</v>
       </c>
       <c r="C124" t="s">
-        <v>258</v>
+        <v>448</v>
       </c>
       <c r="D124" t="s">
         <v>258</v>
@@ -4722,7 +4747,7 @@
       </c>
       <c r="H124" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
@@ -4757,7 +4782,7 @@
         <v>261</v>
       </c>
       <c r="C126" t="s">
-        <v>262</v>
+        <v>450</v>
       </c>
       <c r="D126" t="s">
         <v>262</v>
@@ -4770,7 +4795,7 @@
       </c>
       <c r="H126" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.25">
@@ -4781,7 +4806,7 @@
         <v>263</v>
       </c>
       <c r="C127" t="s">
-        <v>264</v>
+        <v>451</v>
       </c>
       <c r="D127" t="s">
         <v>264</v>
@@ -4794,7 +4819,7 @@
       </c>
       <c r="H127" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
@@ -4805,7 +4830,7 @@
         <v>265</v>
       </c>
       <c r="C128" t="s">
-        <v>266</v>
+        <v>452</v>
       </c>
       <c r="D128" t="s">
         <v>266</v>
@@ -4818,7 +4843,7 @@
       </c>
       <c r="H128" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.25">
@@ -4829,7 +4854,7 @@
         <v>267</v>
       </c>
       <c r="C129" t="s">
-        <v>268</v>
+        <v>453</v>
       </c>
       <c r="D129" t="s">
         <v>268</v>
@@ -4842,7 +4867,7 @@
       </c>
       <c r="H129" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.25">
@@ -4853,7 +4878,7 @@
         <v>269</v>
       </c>
       <c r="C130" t="s">
-        <v>270</v>
+        <v>454</v>
       </c>
       <c r="D130" t="s">
         <v>270</v>
@@ -4866,7 +4891,7 @@
       </c>
       <c r="H130" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.25">
@@ -5224,4 +5249,18 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P16" sqref="P16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update number of visits for hr need calculation for ART and second-line ART interventions
</commit_message>
<xml_diff>
--- a/2_data/new_intervention_names.xlsx
+++ b/2_data/new_intervention_names.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="455">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="456">
   <si>
     <t>Category</t>
   </si>
@@ -1393,6 +1393,9 @@
   </si>
   <si>
     <t>Modern contraception: Male sterilization</t>
+  </si>
+  <si>
+    <t>Substance use disorder (alcohol) - Brief advice on alcohol use in primary care including education and psychosocial counselling</t>
   </si>
 </sst>
 </file>
@@ -1759,8 +1762,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B115" workbookViewId="0">
-      <selection activeCell="C127" sqref="C127"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4494,7 +4497,7 @@
         <v>235</v>
       </c>
       <c r="C114" t="s">
-        <v>236</v>
+        <v>455</v>
       </c>
       <c r="D114" t="s">
         <v>236</v>
@@ -4507,7 +4510,7 @@
       </c>
       <c r="H114" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
series of commits before drafting responses
</commit_message>
<xml_diff>
--- a/2_data/new_intervention_names.xlsx
+++ b/2_data/new_intervention_names.xlsx
@@ -1,34 +1,46 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sm2511\Dropbox\York\Research Projects\Uganda EHP\Analysis\repo\uganda_hbp\2_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1A7D4FE-D29C-4C12-9F02-1B9EFB7C474D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="10065"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$144</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$147</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="456">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="462">
   <si>
     <t>Category</t>
   </si>
@@ -1396,13 +1408,31 @@
   </si>
   <si>
     <t>Substance use disorder (alcohol) - Brief advice on alcohol use in primary care including education and psychosocial counselling</t>
+  </si>
+  <si>
+    <t>350</t>
+  </si>
+  <si>
+    <t>351</t>
+  </si>
+  <si>
+    <t>352</t>
+  </si>
+  <si>
+    <t>353</t>
+  </si>
+  <si>
+    <t>Vaginal delivery (with and without complication)</t>
+  </si>
+  <si>
+    <t>354</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1413,6 +1443,12 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1432,7 +1468,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -1440,38 +1476,22 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3 2 2" xfId="1"/>
+    <cellStyle name="Normal 3 2 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -1759,23 +1779,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:H147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="42" customWidth="1"/>
+    <col min="3" max="3" width="65.08984375" customWidth="1"/>
     <col min="4" max="4" width="47" customWidth="1"/>
-    <col min="5" max="5" width="27.28515625" customWidth="1"/>
-    <col min="7" max="7" width="7.42578125" customWidth="1"/>
-    <col min="8" max="8" width="30.140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="27.26953125" customWidth="1"/>
+    <col min="7" max="7" width="7.453125" customWidth="1"/>
+    <col min="8" max="8" width="30.1796875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1798,7 +1819,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1822,7 +1843,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1846,7 +1867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1870,7 +1891,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1894,7 +1915,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -1918,7 +1939,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -1942,7 +1963,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -1966,7 +1987,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -1990,7 +2011,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -2014,7 +2035,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -2041,7 +2062,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -2065,7 +2086,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -2089,7 +2110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -2113,14 +2134,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>3</v>
       </c>
       <c r="B15" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="3" t="s">
         <v>31</v>
       </c>
       <c r="D15" t="s">
@@ -2137,7 +2158,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -2161,7 +2182,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>3</v>
       </c>
@@ -2185,14 +2206,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>3</v>
       </c>
       <c r="B18" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="3" t="s">
         <v>37</v>
       </c>
       <c r="D18" t="s">
@@ -2209,7 +2230,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>3</v>
       </c>
@@ -2233,7 +2254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>3</v>
       </c>
@@ -2257,14 +2278,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>3</v>
       </c>
       <c r="B21" t="s">
         <v>42</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="3" t="s">
         <v>43</v>
       </c>
       <c r="D21" t="s">
@@ -2281,7 +2302,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>3</v>
       </c>
@@ -2305,7 +2326,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>3</v>
       </c>
@@ -2329,7 +2350,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>3</v>
       </c>
@@ -2353,7 +2374,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>3</v>
       </c>
@@ -2377,7 +2398,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>3</v>
       </c>
@@ -2401,7 +2422,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>3</v>
       </c>
@@ -2425,7 +2446,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>56</v>
       </c>
@@ -2449,7 +2470,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>56</v>
       </c>
@@ -2473,7 +2494,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>56</v>
       </c>
@@ -2497,7 +2518,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>56</v>
       </c>
@@ -2521,7 +2542,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>65</v>
       </c>
@@ -2545,7 +2566,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>65</v>
       </c>
@@ -2569,7 +2590,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>65</v>
       </c>
@@ -2593,7 +2614,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>65</v>
       </c>
@@ -2617,7 +2638,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>65</v>
       </c>
@@ -2641,7 +2662,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>65</v>
       </c>
@@ -2665,7 +2686,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>65</v>
       </c>
@@ -2689,7 +2710,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>65</v>
       </c>
@@ -2713,7 +2734,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>3</v>
       </c>
@@ -2737,7 +2758,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>65</v>
       </c>
@@ -2761,7 +2782,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>65</v>
       </c>
@@ -2785,7 +2806,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>88</v>
       </c>
@@ -2809,7 +2830,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>88</v>
       </c>
@@ -2833,7 +2854,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>88</v>
       </c>
@@ -2857,7 +2878,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>88</v>
       </c>
@@ -2881,7 +2902,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>88</v>
       </c>
@@ -2905,7 +2926,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>88</v>
       </c>
@@ -2929,7 +2950,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>88</v>
       </c>
@@ -2953,7 +2974,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>88</v>
       </c>
@@ -2977,7 +2998,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>88</v>
       </c>
@@ -3001,7 +3022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>88</v>
       </c>
@@ -3025,7 +3046,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>109</v>
       </c>
@@ -3049,7 +3070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>109</v>
       </c>
@@ -3073,7 +3094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>109</v>
       </c>
@@ -3097,7 +3118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>109</v>
       </c>
@@ -3121,7 +3142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>109</v>
       </c>
@@ -3145,7 +3166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>109</v>
       </c>
@@ -3169,7 +3190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>109</v>
       </c>
@@ -3193,7 +3214,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>109</v>
       </c>
@@ -3217,7 +3238,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>56</v>
       </c>
@@ -3241,7 +3262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>56</v>
       </c>
@@ -3265,7 +3286,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>56</v>
       </c>
@@ -3289,7 +3310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>56</v>
       </c>
@@ -3313,7 +3334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>56</v>
       </c>
@@ -3337,7 +3358,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>56</v>
       </c>
@@ -3361,7 +3382,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>56</v>
       </c>
@@ -3385,7 +3406,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>56</v>
       </c>
@@ -3409,7 +3430,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>56</v>
       </c>
@@ -3433,7 +3454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>56</v>
       </c>
@@ -3457,7 +3478,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>56</v>
       </c>
@@ -3481,7 +3502,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>56</v>
       </c>
@@ -3505,7 +3526,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>56</v>
       </c>
@@ -3529,7 +3550,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>56</v>
       </c>
@@ -3553,7 +3574,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>56</v>
       </c>
@@ -3577,7 +3598,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>56</v>
       </c>
@@ -3601,7 +3622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>56</v>
       </c>
@@ -3625,7 +3646,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>56</v>
       </c>
@@ -3649,7 +3670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>162</v>
       </c>
@@ -3673,7 +3694,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>162</v>
       </c>
@@ -3697,7 +3718,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>162</v>
       </c>
@@ -3721,7 +3742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>162</v>
       </c>
@@ -3745,7 +3766,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>162</v>
       </c>
@@ -3769,7 +3790,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>162</v>
       </c>
@@ -3793,7 +3814,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>162</v>
       </c>
@@ -3817,7 +3838,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>177</v>
       </c>
@@ -3841,7 +3862,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>177</v>
       </c>
@@ -3865,7 +3886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>177</v>
       </c>
@@ -3889,7 +3910,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>177</v>
       </c>
@@ -3913,7 +3934,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>177</v>
       </c>
@@ -3937,7 +3958,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>177</v>
       </c>
@@ -3961,7 +3982,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>177</v>
       </c>
@@ -3985,7 +4006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>177</v>
       </c>
@@ -4009,7 +4030,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>177</v>
       </c>
@@ -4033,7 +4054,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>177</v>
       </c>
@@ -4057,7 +4078,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>177</v>
       </c>
@@ -4081,7 +4102,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>177</v>
       </c>
@@ -4105,7 +4126,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>177</v>
       </c>
@@ -4129,7 +4150,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>177</v>
       </c>
@@ -4153,7 +4174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>177</v>
       </c>
@@ -4177,7 +4198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>177</v>
       </c>
@@ -4201,7 +4222,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>177</v>
       </c>
@@ -4225,7 +4246,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>177</v>
       </c>
@@ -4249,7 +4270,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>177</v>
       </c>
@@ -4273,7 +4294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>177</v>
       </c>
@@ -4297,7 +4318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>177</v>
       </c>
@@ -4321,7 +4342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>177</v>
       </c>
@@ -4345,7 +4366,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>222</v>
       </c>
@@ -4369,7 +4390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>222</v>
       </c>
@@ -4393,7 +4414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>222</v>
       </c>
@@ -4417,7 +4438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>222</v>
       </c>
@@ -4441,7 +4462,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>222</v>
       </c>
@@ -4465,7 +4486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>222</v>
       </c>
@@ -4489,7 +4510,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>177</v>
       </c>
@@ -4513,7 +4534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>237</v>
       </c>
@@ -4537,7 +4558,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>237</v>
       </c>
@@ -4561,7 +4582,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>237</v>
       </c>
@@ -4585,7 +4606,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>244</v>
       </c>
@@ -4609,7 +4630,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>244</v>
       </c>
@@ -4633,7 +4654,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>244</v>
       </c>
@@ -4657,7 +4678,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>244</v>
       </c>
@@ -4681,7 +4702,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>3</v>
       </c>
@@ -4705,7 +4726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>3</v>
       </c>
@@ -4729,7 +4750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>3</v>
       </c>
@@ -4753,7 +4774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>3</v>
       </c>
@@ -4777,7 +4798,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>3</v>
       </c>
@@ -4801,7 +4822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>3</v>
       </c>
@@ -4825,7 +4846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>3</v>
       </c>
@@ -4849,7 +4870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>3</v>
       </c>
@@ -4873,7 +4894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
         <v>3</v>
       </c>
@@ -4897,7 +4918,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
         <v>3</v>
       </c>
@@ -4921,7 +4942,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
         <v>162</v>
       </c>
@@ -4945,7 +4966,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>162</v>
       </c>
@@ -4969,7 +4990,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
         <v>109</v>
       </c>
@@ -4993,7 +5014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
         <v>109</v>
       </c>
@@ -5017,7 +5038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
         <v>56</v>
       </c>
@@ -5041,7 +5062,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
         <v>56</v>
       </c>
@@ -5065,7 +5086,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
         <v>162</v>
       </c>
@@ -5089,7 +5110,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
         <v>177</v>
       </c>
@@ -5113,7 +5134,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>3</v>
       </c>
@@ -5137,7 +5158,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
         <v>3</v>
       </c>
@@ -5161,7 +5182,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
         <v>65</v>
       </c>
@@ -5185,14 +5206,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B143">
-        <v>350</v>
-      </c>
-      <c r="C143" s="3" t="s">
+    <row r="143" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="B143" t="s">
+        <v>456</v>
+      </c>
+      <c r="C143" t="s">
         <v>434</v>
       </c>
-      <c r="D143" s="3" t="s">
+      <c r="D143" t="s">
         <v>434</v>
       </c>
       <c r="H143" t="b">
@@ -5200,14 +5221,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B144">
-        <v>351</v>
-      </c>
-      <c r="C144" s="3" t="s">
+    <row r="144" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="B144" t="s">
+        <v>457</v>
+      </c>
+      <c r="C144" t="s">
         <v>435</v>
       </c>
-      <c r="D144" s="3" t="s">
+      <c r="D144" t="s">
         <v>435</v>
       </c>
       <c r="H144" t="b">
@@ -5215,39 +5236,61 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="B145" t="s">
+        <v>458</v>
+      </c>
+      <c r="C145" t="s">
+        <v>460</v>
+      </c>
+      <c r="D145" t="s">
+        <v>460</v>
+      </c>
       <c r="H145" t="b">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B146">
-        <v>353</v>
-      </c>
-      <c r="C146" s="1" t="s">
+    <row r="146" spans="2:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="B146" t="s">
+        <v>459</v>
+      </c>
+      <c r="C146" t="s">
+        <v>445</v>
+      </c>
+      <c r="D146" t="s">
         <v>445</v>
       </c>
       <c r="H146" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="147" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B147">
-        <v>354</v>
-      </c>
-      <c r="C147" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147" spans="2:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="B147" t="s">
+        <v>461</v>
+      </c>
+      <c r="C147" t="s">
+        <v>446</v>
+      </c>
+      <c r="D147" t="s">
         <v>446</v>
       </c>
       <c r="H147" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H144"/>
-  <conditionalFormatting sqref="F1:F1048576 G11">
+  <autoFilter ref="A1:H147" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <filterColumn colId="7">
+      <filters>
+        <filter val="FALSE"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <conditionalFormatting sqref="G11 F1:F1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5255,14 +5298,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>